<commit_message>
after Averta madness, means in q_fpca... CARE!
</commit_message>
<xml_diff>
--- a/Data Analysis/00_Immagini, idee/ParticipantCharacteristics.xlsx
+++ b/Data Analysis/00_Immagini, idee/ParticipantCharacteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrea Ferroni\Google Drive\Robotica\Data Analysis\File Matlab\tabelle, disegni altro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\rob_upperlimb_strokes\Data Analysis\00_Immagini, idee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C1756D-9F1B-4A26-B1FB-1A9E478D826C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EED5DD-716E-48D4-A8B1-475A191081ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="750" windowWidth="16740" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PartChar" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
   <si>
     <t>Patient-ID</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>59.14 ±15.85</t>
+  </si>
+  <si>
+    <t>CANCELLATO</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>subj studiati da averta</t>
   </si>
 </sst>
 </file>
@@ -193,7 +202,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +212,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -304,9 +319,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -589,8 +611,8 @@
   </sheetPr>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -599,6 +621,7 @@
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="5" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -623,7 +646,9 @@
       <c r="G1" s="3">
         <v>54</v>
       </c>
-      <c r="H1"/>
+      <c r="H1" s="5">
+        <v>6</v>
+      </c>
       <c r="N1"/>
       <c r="O1"/>
       <c r="P1"/>
@@ -654,6 +679,9 @@
       <c r="G2" s="3">
         <v>55</v>
       </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -677,9 +705,12 @@
       <c r="G3" s="3">
         <v>55</v>
       </c>
+      <c r="H3" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -699,6 +730,9 @@
       </c>
       <c r="G4" s="3">
         <v>38</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -723,6 +757,9 @@
       <c r="G5" s="3">
         <v>41</v>
       </c>
+      <c r="H5" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -746,9 +783,16 @@
       <c r="G6" s="3">
         <v>47</v>
       </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -769,9 +813,12 @@
       <c r="G7" s="3">
         <v>40</v>
       </c>
+      <c r="H7" s="5">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -791,6 +838,9 @@
       </c>
       <c r="G8" s="3">
         <v>49</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -815,9 +865,12 @@
       <c r="G9" s="3">
         <v>43</v>
       </c>
+      <c r="H9" s="5">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -838,9 +891,12 @@
       <c r="G10" s="3">
         <v>37</v>
       </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -860,6 +916,9 @@
       </c>
       <c r="G11" s="3">
         <v>53</v>
+      </c>
+      <c r="H11" s="5">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -884,9 +943,12 @@
       <c r="G12" s="3">
         <v>59</v>
       </c>
+      <c r="H12">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -906,6 +968,9 @@
       </c>
       <c r="G13" s="3">
         <v>37</v>
+      </c>
+      <c r="H13" s="5">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -930,6 +995,9 @@
       <c r="G14" s="3">
         <v>61</v>
       </c>
+      <c r="H14">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -953,6 +1021,9 @@
       <c r="G15" s="3">
         <v>42</v>
       </c>
+      <c r="H15" s="5">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -976,6 +1047,9 @@
       <c r="G16" s="3">
         <v>48</v>
       </c>
+      <c r="H16">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -999,6 +1073,9 @@
       <c r="G17" s="3">
         <v>60</v>
       </c>
+      <c r="H17" s="5">
+        <v>22</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1022,6 +1099,9 @@
       <c r="G18" s="3">
         <v>34</v>
       </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1045,6 +1125,9 @@
       <c r="G19" s="3">
         <v>46</v>
       </c>
+      <c r="H19" s="5">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1067,6 +1150,9 @@
       </c>
       <c r="G20" s="3">
         <v>21</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
analysis of reconstruction error plots
</commit_message>
<xml_diff>
--- a/Data Analysis/00_Immagini, idee/ParticipantCharacteristics.xlsx
+++ b/Data Analysis/00_Immagini, idee/ParticipantCharacteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\rob_upperlimb_strokes\Data Analysis\00_Immagini, idee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EED5DD-716E-48D4-A8B1-475A191081ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285A65E0-B20F-4A6A-B4FB-6FF6C1218466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="2745" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PartChar" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
   <si>
     <t>Patient-ID</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>CANCELLATO</t>
-  </si>
-  <si>
-    <t>()</t>
   </si>
   <si>
     <t>subj studiati da averta</t>
@@ -612,7 +609,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -788,7 +785,7 @@
       </c>
       <c r="L6" s="14"/>
       <c r="M6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1151,8 +1148,8 @@
       <c r="G20" s="3">
         <v>21</v>
       </c>
-      <c r="H20" t="s">
-        <v>44</v>
+      <c r="H20">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
plot var and mean of rec error
</commit_message>
<xml_diff>
--- a/Data Analysis/00_Immagini, idee/ParticipantCharacteristics.xlsx
+++ b/Data Analysis/00_Immagini, idee/ParticipantCharacteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\rob_upperlimb_strokes\Data Analysis\00_Immagini, idee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285A65E0-B20F-4A6A-B4FB-6FF6C1218466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4170008-2B2A-4A0A-9DE9-C9A7E3935334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="2745" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="2220" windowWidth="15300" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PartChar" sheetId="1" r:id="rId1"/>
@@ -283,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -323,6 +323,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,7 +612,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1096,7 +1099,7 @@
       <c r="G18" s="3">
         <v>34</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="15" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update Reconstruct Error, single joints
</commit_message>
<xml_diff>
--- a/Data Analysis/00_Immagini, idee/ParticipantCharacteristics.xlsx
+++ b/Data Analysis/00_Immagini, idee/ParticipantCharacteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\rob_upperlimb_strokes\Data Analysis\00_Immagini, idee\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4170008-2B2A-4A0A-9DE9-C9A7E3935334}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EF0838F-7E8D-4991-A16F-7B2DFCC0DA16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2220" windowWidth="15300" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="14220" yWindow="2130" windowWidth="15300" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PartChar" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
   <si>
     <t>Patient-ID</t>
   </si>
@@ -159,7 +159,10 @@
     <t>CANCELLATO</t>
   </si>
   <si>
-    <t>subj studiati da averta</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -199,7 +202,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -313,18 +322,40 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,8 +642,8 @@
   </sheetPr>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -625,25 +656,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="5" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3">
+      <c r="B1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="18">
         <v>55</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="18">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="18">
         <v>54</v>
       </c>
       <c r="H1" s="5">
@@ -658,25 +689,25 @@
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14">
         <v>55</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="14">
         <v>24</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="3">
+      <c r="E2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="14">
         <v>55</v>
       </c>
       <c r="H2">
@@ -684,25 +715,25 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="14">
         <v>52</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="14">
         <v>34</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="14">
         <v>55</v>
       </c>
       <c r="H3" s="5">
@@ -710,25 +741,25 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="14">
         <v>73</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="14">
         <v>18</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="E4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="14">
         <v>38</v>
       </c>
       <c r="H4">
@@ -736,25 +767,25 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="18">
         <v>69</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="18">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="18">
         <v>41</v>
       </c>
       <c r="H5" s="5">
@@ -762,81 +793,85 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="15">
         <v>40</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="14">
         <v>9</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="3">
+      <c r="E6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="14">
         <v>47</v>
       </c>
       <c r="H6">
         <v>11</v>
       </c>
-      <c r="L6" s="14"/>
+      <c r="L6" s="12"/>
       <c r="M6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="18">
         <v>71</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="18">
         <v>55</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="E7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="18">
         <v>40</v>
       </c>
       <c r="H7" s="5">
         <v>12</v>
       </c>
+      <c r="L7" s="19"/>
+      <c r="M7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="18">
         <v>58</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="18">
         <v>53</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="E8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="18">
         <v>49</v>
       </c>
       <c r="H8">
@@ -844,25 +879,25 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="14">
         <v>69</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="14">
         <v>6</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="3">
+      <c r="E9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="14">
         <v>43</v>
       </c>
       <c r="H9" s="5">
@@ -870,25 +905,25 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14">
         <v>61</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="14">
         <v>73</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="E10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="14">
         <v>37</v>
       </c>
       <c r="H10">
@@ -896,25 +931,25 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B11" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="18">
         <v>59</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="18">
         <v>20</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="E11" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="18">
         <v>53</v>
       </c>
       <c r="H11" s="5">
@@ -922,25 +957,25 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B12" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="18">
         <v>55</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="18">
         <v>18</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="E12" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="18">
         <v>59</v>
       </c>
       <c r="H12">
@@ -948,25 +983,25 @@
       </c>
     </row>
     <row r="13" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="18">
         <v>42</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="18">
         <v>6</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="18">
         <v>37</v>
       </c>
       <c r="H13" s="5">
@@ -974,25 +1009,25 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="14">
         <v>51</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="14">
         <v>12</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="E14" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="14">
         <v>61</v>
       </c>
       <c r="H14">
@@ -1000,25 +1035,25 @@
       </c>
     </row>
     <row r="15" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="B15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="14">
         <v>58</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="14">
         <v>6</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="E15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="14">
         <v>42</v>
       </c>
       <c r="H15" s="5">
@@ -1026,25 +1061,25 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="B16" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="18">
         <v>78</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="18">
         <v>54</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="E16" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="18">
         <v>48</v>
       </c>
       <c r="H16">
@@ -1052,25 +1087,25 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="3">
+      <c r="B17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="14">
         <v>76</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="14">
         <v>34</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="E17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="14">
         <v>60</v>
       </c>
       <c r="H17" s="5">
@@ -1078,51 +1113,51 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="3">
+      <c r="B18" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="23">
         <v>62</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="23">
         <v>182</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="3">
+      <c r="E18" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="23">
         <v>34</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H18" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="3">
+      <c r="B19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="14">
         <v>62</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="14">
         <v>13</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="E19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="14">
         <v>46</v>
       </c>
       <c r="H19" s="5">
@@ -1130,25 +1165,25 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="14">
         <v>74</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="14">
         <v>12</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="3">
+      <c r="E20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="14">
         <v>21</v>
       </c>
       <c r="H20">

</xml_diff>